<commit_message>
LCD RGB888 display 800*480 4.3
</commit_message>
<xml_diff>
--- a/ART_PI_引脚分布.xlsx
+++ b/ART_PI_引脚分布.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9300"/>
+    <workbookView windowWidth="23040" windowHeight="9300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ART_PI" sheetId="1" r:id="rId1"/>
@@ -2112,8 +2112,8 @@
   <sheetPr/>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -3336,8 +3336,8 @@
   <sheetPr/>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>

</xml_diff>